<commit_message>
Create running forecasting scheme
</commit_message>
<xml_diff>
--- a/Blocks.xlsx
+++ b/Blocks.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sigve Borgmo\MATLAB Drive\Master\dynamic-factor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sigve Borgmo\Master\dynamic-factor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496E7906-B48C-46E3-88E6-EBD1D4E3FF3D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B94597-F582-43FE-AE68-B68FF403A4A8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Block1" sheetId="2" r:id="rId1"/>
     <sheet name="Block2" sheetId="4" r:id="rId2"/>
     <sheet name="Comm2" sheetId="5" r:id="rId3"/>
+    <sheet name="Block3" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="200">
   <si>
     <t>Platinum</t>
   </si>
@@ -348,6 +349,285 @@
   </si>
   <si>
     <t>Feed</t>
+  </si>
+  <si>
+    <t>Feed consumption (tonnes)</t>
+  </si>
+  <si>
+    <t>FeedCon-3</t>
+  </si>
+  <si>
+    <t>FeedCon-6</t>
+  </si>
+  <si>
+    <t>Sea Lice Level</t>
+  </si>
+  <si>
+    <t>SeaLice-3</t>
+  </si>
+  <si>
+    <t>SeaLice-6</t>
+  </si>
+  <si>
+    <t>SeaLice-9</t>
+  </si>
+  <si>
+    <t>SeaLice-12</t>
+  </si>
+  <si>
+    <t>SeaLice-15</t>
+  </si>
+  <si>
+    <t>SeaTemp</t>
+  </si>
+  <si>
+    <t>SeaTemp-3</t>
+  </si>
+  <si>
+    <t>SeaTemp-6</t>
+  </si>
+  <si>
+    <t>SeaTemp-9</t>
+  </si>
+  <si>
+    <t>SeaTemp-12</t>
+  </si>
+  <si>
+    <t>SeaTemp-15</t>
+  </si>
+  <si>
+    <t>Biomass salmon (ton)</t>
+  </si>
+  <si>
+    <t>BiomassSalmon-3</t>
+  </si>
+  <si>
+    <t>BiomassSalmon-6</t>
+  </si>
+  <si>
+    <t>BiomassSalmon-9</t>
+  </si>
+  <si>
+    <t>BiomassSalmon-12</t>
+  </si>
+  <si>
+    <t>BiomassSalmon-15</t>
+  </si>
+  <si>
+    <t>Smolt (antall)</t>
+  </si>
+  <si>
+    <t>Smolt-12</t>
+  </si>
+  <si>
+    <t>Smolt-15</t>
+  </si>
+  <si>
+    <t>Smolt-17</t>
+  </si>
+  <si>
+    <t>Smolt-18</t>
+  </si>
+  <si>
+    <t>Smolt-21</t>
+  </si>
+  <si>
+    <t>ConsEU-3</t>
+  </si>
+  <si>
+    <t>ConsEU-6</t>
+  </si>
+  <si>
+    <t>ConsEU-9</t>
+  </si>
+  <si>
+    <t>ConsEU-12</t>
+  </si>
+  <si>
+    <t>ConsEU-15</t>
+  </si>
+  <si>
+    <t>ConsEM-3</t>
+  </si>
+  <si>
+    <t>ConsEM-6</t>
+  </si>
+  <si>
+    <t>ConsEM-9</t>
+  </si>
+  <si>
+    <t>ConsEM-12</t>
+  </si>
+  <si>
+    <t>ConsEM-15</t>
+  </si>
+  <si>
+    <t>Salmon</t>
+  </si>
+  <si>
+    <t>Salmon-1</t>
+  </si>
+  <si>
+    <t>Salmon-2</t>
+  </si>
+  <si>
+    <t>Salmon-3</t>
+  </si>
+  <si>
+    <t>Salmon-4</t>
+  </si>
+  <si>
+    <t>Salmon-5</t>
+  </si>
+  <si>
+    <t>Salmon-6</t>
+  </si>
+  <si>
+    <t>Salmon-7</t>
+  </si>
+  <si>
+    <t>Salmon-8</t>
+  </si>
+  <si>
+    <t>Salmon-9</t>
+  </si>
+  <si>
+    <t>Salmon-10</t>
+  </si>
+  <si>
+    <t>Salmon-11</t>
+  </si>
+  <si>
+    <t>Salmon-12</t>
+  </si>
+  <si>
+    <t>Shrimp-3</t>
+  </si>
+  <si>
+    <t>Shrimp-6</t>
+  </si>
+  <si>
+    <t>Trout</t>
+  </si>
+  <si>
+    <t>Trout-3</t>
+  </si>
+  <si>
+    <t>Trout-6</t>
+  </si>
+  <si>
+    <t>Cod</t>
+  </si>
+  <si>
+    <t>Cod-6</t>
+  </si>
+  <si>
+    <t>Mea-3</t>
+  </si>
+  <si>
+    <t>Bef-3</t>
+  </si>
+  <si>
+    <t>Bef-6</t>
+  </si>
+  <si>
+    <t>E/N-3</t>
+  </si>
+  <si>
+    <t>E/N-6</t>
+  </si>
+  <si>
+    <t>E/N-9</t>
+  </si>
+  <si>
+    <t>CLP/USD</t>
+  </si>
+  <si>
+    <t>C/U-3</t>
+  </si>
+  <si>
+    <t>C/U-6</t>
+  </si>
+  <si>
+    <t>C/U-9</t>
+  </si>
+  <si>
+    <t>BB-3</t>
+  </si>
+  <si>
+    <t>BB-6</t>
+  </si>
+  <si>
+    <t>BB-9</t>
+  </si>
+  <si>
+    <t>Real I-rate</t>
+  </si>
+  <si>
+    <t>RI-1</t>
+  </si>
+  <si>
+    <t>RI-2</t>
+  </si>
+  <si>
+    <t>RI-3</t>
+  </si>
+  <si>
+    <t>RI-4</t>
+  </si>
+  <si>
+    <t>RI-5</t>
+  </si>
+  <si>
+    <t>RI-6</t>
+  </si>
+  <si>
+    <t>WHE-3</t>
+  </si>
+  <si>
+    <t>WHE-6</t>
+  </si>
+  <si>
+    <t>FH-3</t>
+  </si>
+  <si>
+    <t>FH-6</t>
+  </si>
+  <si>
+    <t>SOYM-3</t>
+  </si>
+  <si>
+    <t>SOYM-6</t>
+  </si>
+  <si>
+    <t>RAP-3</t>
+  </si>
+  <si>
+    <t>RAP-6</t>
+  </si>
+  <si>
+    <t>Corn</t>
+  </si>
+  <si>
+    <t>COR-3</t>
+  </si>
+  <si>
+    <t>COR-6</t>
+  </si>
+  <si>
+    <t>MHG -Eq</t>
+  </si>
+  <si>
+    <t>MHG-1</t>
+  </si>
+  <si>
+    <t>MHG-2</t>
+  </si>
+  <si>
+    <t>MHG-3</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
 </sst>
 </file>
@@ -395,7 +675,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -423,11 +703,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -480,11 +769,41 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -2569,7 +2888,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C60">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>$C1=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2594,8 +2913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D232A71-68CA-4AA6-A86F-03EF34E1AC26}">
   <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3626,7 +3945,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C60">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$C1=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3651,13 +3970,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{169B3490-1409-431C-8AC7-52E7F0D4906B}">
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.109375" style="11" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" style="14" customWidth="1"/>
+    <col min="6" max="11" width="11.33203125" style="14" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11.33203125" style="14" customWidth="1"/>
+    <col min="15" max="15" width="14.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -3671,8 +3997,6 @@
         <f t="shared" ref="C1:C60" si="0">COUNTIF($G$3:$AG$100, A1)</f>
         <v>1</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="14"/>
       <c r="F1" s="15" t="s">
         <v>67</v>
       </c>
@@ -3715,7 +4039,6 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D2" s="12"/>
       <c r="E2" s="16" t="s">
         <v>68</v>
       </c>
@@ -3761,7 +4084,6 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D3" s="12"/>
       <c r="E3" s="18" t="s">
         <v>69</v>
       </c>
@@ -3807,9 +4129,6 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
       <c r="G4" s="19">
         <v>9</v>
       </c>
@@ -3849,9 +4168,6 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
       <c r="G5" s="19">
         <v>10</v>
       </c>
@@ -3889,9 +4205,6 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
       <c r="G6" s="19">
         <v>11</v>
       </c>
@@ -3927,9 +4240,6 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
       <c r="G7" s="19"/>
       <c r="H7" s="19">
         <v>16</v>
@@ -3963,9 +4273,6 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
       <c r="G8" s="19"/>
       <c r="H8" s="19">
         <v>17</v>
@@ -3997,9 +4304,6 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
       <c r="G9" s="19"/>
       <c r="H9" s="19">
         <v>18</v>
@@ -4027,9 +4331,6 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
@@ -4039,7 +4340,6 @@
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
       <c r="M10" s="19"/>
-      <c r="N10" s="14"/>
       <c r="O10" s="19"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -4053,9 +4353,6 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
       <c r="I11" s="19"/>
@@ -4077,18 +4374,6 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
@@ -4101,18 +4386,6 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
@@ -4125,18 +4398,6 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
@@ -4149,18 +4410,6 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
@@ -4173,20 +4422,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D16" s="12"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <v>17</v>
       </c>
@@ -4197,20 +4434,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>18</v>
       </c>
@@ -4221,20 +4446,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>19</v>
       </c>
@@ -4245,20 +4458,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>20</v>
       </c>
@@ -4269,20 +4470,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>21</v>
       </c>
@@ -4293,20 +4482,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>22</v>
       </c>
@@ -4317,20 +4494,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>23</v>
       </c>
@@ -4341,20 +4506,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>24</v>
       </c>
@@ -4365,20 +4518,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>25</v>
       </c>
@@ -4389,20 +4530,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>26</v>
       </c>
@@ -4413,20 +4542,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>27</v>
       </c>
@@ -4437,20 +4554,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>28</v>
       </c>
@@ -4461,20 +4566,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>29</v>
       </c>
@@ -4485,20 +4578,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>30</v>
       </c>
@@ -4509,20 +4590,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D30" s="12"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <v>31</v>
       </c>
@@ -4533,20 +4602,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D31" s="12"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="14"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <v>32</v>
       </c>
@@ -4557,20 +4614,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D32" s="12"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
         <v>33</v>
       </c>
@@ -4581,20 +4626,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D33" s="12"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>34</v>
       </c>
@@ -4605,20 +4638,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D34" s="12"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="14"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>35</v>
       </c>
@@ -4629,20 +4650,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D35" s="12"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
         <v>36</v>
       </c>
@@ -4653,20 +4662,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D36" s="12"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
-      <c r="O36" s="14"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>37</v>
       </c>
@@ -4677,20 +4674,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D37" s="12"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
         <v>38</v>
       </c>
@@ -4701,20 +4686,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D38" s="12"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
         <v>39</v>
       </c>
@@ -4725,20 +4698,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D39" s="12"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="14"/>
-      <c r="L39" s="14"/>
-      <c r="M39" s="14"/>
-      <c r="N39" s="14"/>
-      <c r="O39" s="14"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="13">
         <v>40</v>
       </c>
@@ -4749,20 +4710,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D40" s="12"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="13">
         <v>41</v>
       </c>
@@ -4773,20 +4722,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D41" s="12"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="14"/>
-      <c r="O41" s="14"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="13">
         <v>42</v>
       </c>
@@ -4797,20 +4734,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D42" s="12"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="13">
         <v>43</v>
       </c>
@@ -4821,20 +4746,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D43" s="12"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
         <v>44</v>
       </c>
@@ -4845,20 +4758,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D44" s="12"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="14"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="13">
         <v>45</v>
       </c>
@@ -4869,20 +4770,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D45" s="12"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="14"/>
-      <c r="K45" s="14"/>
-      <c r="L45" s="14"/>
-      <c r="M45" s="14"/>
-      <c r="N45" s="14"/>
-      <c r="O45" s="14"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="13">
         <v>46</v>
       </c>
@@ -4893,20 +4782,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D46" s="12"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="14"/>
-      <c r="K46" s="14"/>
-      <c r="L46" s="14"/>
-      <c r="M46" s="14"/>
-      <c r="N46" s="14"/>
-      <c r="O46" s="14"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="13">
         <v>47</v>
       </c>
@@ -4917,20 +4794,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D47" s="12"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="14"/>
-      <c r="K47" s="14"/>
-      <c r="L47" s="14"/>
-      <c r="M47" s="14"/>
-      <c r="N47" s="14"/>
-      <c r="O47" s="14"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="13">
         <v>48</v>
       </c>
@@ -4941,20 +4806,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D48" s="12"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
-      <c r="J48" s="14"/>
-      <c r="K48" s="14"/>
-      <c r="L48" s="14"/>
-      <c r="M48" s="14"/>
-      <c r="N48" s="14"/>
-      <c r="O48" s="14"/>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
         <v>49</v>
       </c>
@@ -4965,20 +4818,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D49" s="12"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="14"/>
-      <c r="K49" s="14"/>
-      <c r="L49" s="14"/>
-      <c r="M49" s="14"/>
-      <c r="N49" s="14"/>
-      <c r="O49" s="14"/>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="13">
         <v>50</v>
       </c>
@@ -4989,20 +4830,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D50" s="12"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="14"/>
-      <c r="L50" s="14"/>
-      <c r="M50" s="14"/>
-      <c r="N50" s="14"/>
-      <c r="O50" s="14"/>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="13">
         <v>51</v>
       </c>
@@ -5013,20 +4842,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D51" s="12"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14"/>
-      <c r="L51" s="14"/>
-      <c r="M51" s="14"/>
-      <c r="N51" s="14"/>
-      <c r="O51" s="14"/>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="13">
         <v>52</v>
       </c>
@@ -5037,20 +4854,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D52" s="12"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="14"/>
-      <c r="L52" s="14"/>
-      <c r="M52" s="14"/>
-      <c r="N52" s="14"/>
-      <c r="O52" s="14"/>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="13">
         <v>53</v>
       </c>
@@ -5061,20 +4866,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D53" s="12"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
-      <c r="J53" s="14"/>
-      <c r="K53" s="14"/>
-      <c r="L53" s="14"/>
-      <c r="M53" s="14"/>
-      <c r="N53" s="14"/>
-      <c r="O53" s="14"/>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="13">
         <v>54</v>
       </c>
@@ -5085,20 +4878,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D54" s="12"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="14"/>
-      <c r="K54" s="14"/>
-      <c r="L54" s="14"/>
-      <c r="M54" s="14"/>
-      <c r="N54" s="14"/>
-      <c r="O54" s="14"/>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="13">
         <v>55</v>
       </c>
@@ -5109,20 +4890,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D55" s="12"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="14"/>
-      <c r="K55" s="14"/>
-      <c r="L55" s="14"/>
-      <c r="M55" s="14"/>
-      <c r="N55" s="14"/>
-      <c r="O55" s="14"/>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="13">
         <v>56</v>
       </c>
@@ -5133,20 +4902,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D56" s="12"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
-      <c r="J56" s="14"/>
-      <c r="K56" s="14"/>
-      <c r="L56" s="14"/>
-      <c r="M56" s="14"/>
-      <c r="N56" s="14"/>
-      <c r="O56" s="14"/>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="13">
         <v>57</v>
       </c>
@@ -5155,20 +4912,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D57" s="12"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="14"/>
-      <c r="K57" s="14"/>
-      <c r="L57" s="14"/>
-      <c r="M57" s="14"/>
-      <c r="N57" s="14"/>
-      <c r="O57" s="14"/>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="13">
         <v>58</v>
       </c>
@@ -5177,20 +4922,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D58" s="12"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="14"/>
-      <c r="J58" s="14"/>
-      <c r="K58" s="14"/>
-      <c r="L58" s="14"/>
-      <c r="M58" s="14"/>
-      <c r="N58" s="14"/>
-      <c r="O58" s="14"/>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="13">
         <v>59</v>
       </c>
@@ -5199,20 +4932,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D59" s="12"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="14"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14"/>
-      <c r="I59" s="14"/>
-      <c r="J59" s="14"/>
-      <c r="K59" s="14"/>
-      <c r="L59" s="14"/>
-      <c r="M59" s="14"/>
-      <c r="N59" s="14"/>
-      <c r="O59" s="14"/>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="13">
         <v>60</v>
       </c>
@@ -5221,22 +4942,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D60" s="12"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="14"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
-      <c r="I60" s="14"/>
-      <c r="J60" s="14"/>
-      <c r="K60" s="14"/>
-      <c r="L60" s="14"/>
-      <c r="M60" s="14"/>
-      <c r="N60" s="14"/>
-      <c r="O60" s="14"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C60">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$C1=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5254,4 +4963,1769 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F334363A-B91B-4098-BBC7-2EAA8D3856A9}">
+  <dimension ref="A1:U103"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.109375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="4.77734375" style="22" customWidth="1"/>
+    <col min="4" max="4" width="1.33203125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" style="29" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="28" customWidth="1"/>
+    <col min="8" max="9" width="16.6640625" style="12" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" style="12" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" style="12" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" style="12" customWidth="1"/>
+    <col min="13" max="13" width="11.88671875" style="12" customWidth="1"/>
+    <col min="14" max="14" width="8.77734375" style="12" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" style="12" customWidth="1"/>
+    <col min="16" max="16" width="10.5546875" style="12" customWidth="1"/>
+    <col min="17" max="17" width="8" style="12" customWidth="1"/>
+    <col min="18" max="18" width="15.21875" style="12" customWidth="1"/>
+    <col min="19" max="16384" width="8.88671875" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13">
+        <v>1</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="21">
+        <f>COUNTIF($F$3:$AJ$100, A1)</f>
+        <v>2</v>
+      </c>
+      <c r="D1" s="11"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+    </row>
+    <row r="2" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="24">
+        <v>2</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="21">
+        <f>COUNTIF($F$3:$AJ$100, A2)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="25"/>
+      <c r="E2" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="17">
+        <v>12</v>
+      </c>
+      <c r="G2" s="17">
+        <v>12</v>
+      </c>
+      <c r="H2" s="17">
+        <v>12</v>
+      </c>
+      <c r="I2" s="17">
+        <v>12</v>
+      </c>
+      <c r="J2" s="17">
+        <v>12</v>
+      </c>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
+    </row>
+    <row r="3" spans="1:21" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>3</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="21">
+        <f t="shared" ref="C3:C66" si="0">COUNTIF($F$3:$AJ$100, A3)</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="19">
+        <v>40</v>
+      </c>
+      <c r="H3" s="19">
+        <v>40</v>
+      </c>
+      <c r="I3" s="19">
+        <v>40</v>
+      </c>
+      <c r="J3" s="19">
+        <v>40</v>
+      </c>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+    </row>
+    <row r="4" spans="1:21" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>4</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19">
+        <v>1</v>
+      </c>
+      <c r="H4" s="19">
+        <v>41</v>
+      </c>
+      <c r="I4" s="19">
+        <v>6</v>
+      </c>
+      <c r="J4" s="19">
+        <v>88</v>
+      </c>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+    </row>
+    <row r="5" spans="1:21" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>5</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19">
+        <v>5</v>
+      </c>
+      <c r="H5" s="19">
+        <v>52</v>
+      </c>
+      <c r="I5" s="19">
+        <v>11</v>
+      </c>
+      <c r="J5" s="19">
+        <v>94</v>
+      </c>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+    </row>
+    <row r="6" spans="1:21" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>6</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="21">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19">
+        <v>6</v>
+      </c>
+      <c r="H6" s="19">
+        <v>56</v>
+      </c>
+      <c r="I6" s="19">
+        <v>16</v>
+      </c>
+      <c r="J6" s="19">
+        <v>91</v>
+      </c>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+    </row>
+    <row r="7" spans="1:21" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>7</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19">
+        <v>11</v>
+      </c>
+      <c r="H7" s="19">
+        <v>100</v>
+      </c>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19">
+        <v>1</v>
+      </c>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+    </row>
+    <row r="8" spans="1:21" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>8</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19">
+        <v>13</v>
+      </c>
+      <c r="H8" s="19">
+        <v>101</v>
+      </c>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+    </row>
+    <row r="9" spans="1:21" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <v>9</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19">
+        <v>15</v>
+      </c>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+    </row>
+    <row r="10" spans="1:21" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>10</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19">
+        <v>16</v>
+      </c>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="R10" s="19"/>
+    </row>
+    <row r="11" spans="1:21" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
+        <v>11</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="21">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19">
+        <v>20</v>
+      </c>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+    </row>
+    <row r="12" spans="1:21" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
+        <v>12</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19">
+        <v>25</v>
+      </c>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+    </row>
+    <row r="13" spans="1:21" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
+        <v>13</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" s="21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+    </row>
+    <row r="14" spans="1:21" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <v>14</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+    </row>
+    <row r="15" spans="1:21" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="13">
+        <v>15</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+    </row>
+    <row r="16" spans="1:21" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
+        <v>16</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" s="21">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+    </row>
+    <row r="17" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13">
+        <v>17</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D17" s="11"/>
+      <c r="E17" s="18"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+    </row>
+    <row r="18" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13">
+        <v>18</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="18"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+    </row>
+    <row r="19" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
+        <v>19</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="18"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+    </row>
+    <row r="20" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13">
+        <v>20</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" s="21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="18"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+    </row>
+    <row r="21" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13">
+        <v>21</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C21" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D21" s="11"/>
+      <c r="E21" s="18"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+    </row>
+    <row r="22" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
+        <v>22</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C22" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="18"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+    </row>
+    <row r="23" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="13">
+        <v>23</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C23" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="11"/>
+      <c r="E23" s="18"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+    </row>
+    <row r="24" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="13">
+        <v>24</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D24" s="11"/>
+      <c r="E24" s="18"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+    </row>
+    <row r="25" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13">
+        <v>25</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C25" s="21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D25" s="11"/>
+      <c r="E25" s="18"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+    </row>
+    <row r="26" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13">
+        <v>26</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D26" s="11"/>
+      <c r="E26" s="18"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+    </row>
+    <row r="27" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="13">
+        <v>27</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="C27" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="18"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="12"/>
+    </row>
+    <row r="28" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="13">
+        <v>28</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D28" s="11"/>
+      <c r="E28" s="18"/>
+      <c r="G28" s="19"/>
+      <c r="I28" s="19"/>
+    </row>
+    <row r="29" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="13">
+        <v>29</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="C29" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D29" s="11"/>
+      <c r="E29" s="18"/>
+      <c r="G29" s="19"/>
+    </row>
+    <row r="30" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="13">
+        <v>30</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C30" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D30" s="11"/>
+      <c r="E30" s="18"/>
+      <c r="G30" s="19"/>
+    </row>
+    <row r="31" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="13">
+        <v>31</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C31" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D31" s="11"/>
+      <c r="E31" s="18"/>
+      <c r="G31" s="19"/>
+    </row>
+    <row r="32" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="13">
+        <v>32</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="C32" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D32" s="11"/>
+      <c r="E32" s="18"/>
+      <c r="G32" s="19"/>
+    </row>
+    <row r="33" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="13">
+        <v>33</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C33" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D33" s="11"/>
+      <c r="E33" s="18"/>
+      <c r="G33" s="19"/>
+    </row>
+    <row r="34" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="13">
+        <v>34</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="11"/>
+      <c r="E34" s="18"/>
+      <c r="G34" s="19"/>
+    </row>
+    <row r="35" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13">
+        <v>35</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D35" s="11"/>
+      <c r="E35" s="18"/>
+      <c r="G35" s="19"/>
+    </row>
+    <row r="36" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="13">
+        <v>36</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="C36" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D36" s="11"/>
+      <c r="E36" s="18"/>
+      <c r="G36" s="19"/>
+    </row>
+    <row r="37" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="13">
+        <v>37</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C37" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D37" s="11"/>
+      <c r="E37" s="18"/>
+      <c r="G37" s="19"/>
+    </row>
+    <row r="38" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="13">
+        <v>38</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D38" s="11"/>
+      <c r="E38" s="18"/>
+      <c r="G38" s="19"/>
+    </row>
+    <row r="39" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="13">
+        <v>39</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C39" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D39" s="11"/>
+      <c r="E39" s="18"/>
+      <c r="G39" s="19"/>
+    </row>
+    <row r="40" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="13">
+        <v>40</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="C40" s="21">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D40" s="11"/>
+      <c r="E40" s="18"/>
+      <c r="G40" s="19"/>
+    </row>
+    <row r="41" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="13">
+        <v>41</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C41" s="21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D41" s="11"/>
+      <c r="E41" s="18"/>
+      <c r="G41" s="19"/>
+    </row>
+    <row r="42" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="13">
+        <v>42</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C42" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D42" s="11"/>
+      <c r="E42" s="18"/>
+      <c r="G42" s="19"/>
+    </row>
+    <row r="43" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="13">
+        <v>43</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="C43" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D43" s="11"/>
+      <c r="E43" s="18"/>
+      <c r="G43" s="19"/>
+    </row>
+    <row r="44" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="13">
+        <v>44</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C44" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D44" s="11"/>
+      <c r="E44" s="18"/>
+      <c r="G44" s="19"/>
+    </row>
+    <row r="45" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="13">
+        <v>45</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="C45" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D45" s="11"/>
+      <c r="E45" s="18"/>
+      <c r="G45" s="19"/>
+    </row>
+    <row r="46" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="13">
+        <v>46</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C46" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D46" s="11"/>
+      <c r="E46" s="18"/>
+      <c r="G46" s="19"/>
+    </row>
+    <row r="47" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="13">
+        <v>47</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C47" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D47" s="11"/>
+      <c r="E47" s="18"/>
+      <c r="G47" s="19"/>
+    </row>
+    <row r="48" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="13">
+        <v>48</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C48" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D48" s="11"/>
+      <c r="E48" s="18"/>
+      <c r="G48" s="19"/>
+    </row>
+    <row r="49" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="13">
+        <v>49</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C49" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D49" s="11"/>
+      <c r="E49" s="18"/>
+      <c r="G49" s="19"/>
+    </row>
+    <row r="50" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="13">
+        <v>50</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="C50" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D50" s="11"/>
+      <c r="E50" s="18"/>
+      <c r="G50" s="19"/>
+    </row>
+    <row r="51" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="13">
+        <v>51</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="C51" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D51" s="11"/>
+      <c r="E51" s="18"/>
+      <c r="G51" s="19"/>
+    </row>
+    <row r="52" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="13">
+        <v>52</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C52" s="21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D52" s="11"/>
+      <c r="E52" s="18"/>
+      <c r="G52" s="19"/>
+    </row>
+    <row r="53" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="13">
+        <v>53</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C53" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D53" s="11"/>
+      <c r="E53" s="18"/>
+      <c r="G53" s="19"/>
+    </row>
+    <row r="54" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="13">
+        <v>54</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C54" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D54" s="11"/>
+      <c r="E54" s="18"/>
+      <c r="G54" s="19"/>
+    </row>
+    <row r="55" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="13">
+        <v>55</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="C55" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D55" s="11"/>
+      <c r="E55" s="18"/>
+      <c r="G55" s="19"/>
+    </row>
+    <row r="56" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="13">
+        <v>56</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="C56" s="21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D56" s="11"/>
+      <c r="E56" s="18"/>
+      <c r="G56" s="19"/>
+    </row>
+    <row r="57" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="13">
+        <v>57</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="C57" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D57" s="11"/>
+      <c r="E57" s="18"/>
+      <c r="G57" s="19"/>
+    </row>
+    <row r="58" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="13">
+        <v>58</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="C58" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D58" s="11"/>
+      <c r="E58" s="18"/>
+      <c r="G58" s="19"/>
+    </row>
+    <row r="59" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="13">
+        <v>59</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="C59" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D59" s="11"/>
+      <c r="E59" s="18"/>
+      <c r="G59" s="19"/>
+    </row>
+    <row r="60" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="13">
+        <v>60</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="C60" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D60" s="11"/>
+      <c r="E60" s="18"/>
+      <c r="G60" s="19"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="13">
+        <v>61</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C61" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="13">
+        <v>62</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="C62" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="13">
+        <v>63</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C63" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="13">
+        <v>64</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="C64" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="13">
+        <v>65</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="C65" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="13">
+        <v>66</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C66" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="13">
+        <v>67</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="C67" s="21">
+        <f t="shared" ref="C67:C103" si="1">COUNTIF($F$3:$AJ$100, A67)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="13">
+        <v>68</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="C68" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="13">
+        <v>69</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="C69" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="13">
+        <v>70</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="C70" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="13">
+        <v>71</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="C71" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="13">
+        <v>72</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="C72" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="13">
+        <v>73</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="C73" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="13">
+        <v>74</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C74" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="13">
+        <v>75</v>
+      </c>
+      <c r="B75" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="C75" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="13">
+        <v>76</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="C76" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="13">
+        <v>77</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="C77" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="13">
+        <v>78</v>
+      </c>
+      <c r="B78" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="C78" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="13">
+        <v>79</v>
+      </c>
+      <c r="B79" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="C79" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="13">
+        <v>80</v>
+      </c>
+      <c r="B80" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="C80" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="13">
+        <v>81</v>
+      </c>
+      <c r="B81" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="C81" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="13">
+        <v>82</v>
+      </c>
+      <c r="B82" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="C82" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="13">
+        <v>83</v>
+      </c>
+      <c r="B83" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="C83" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="13">
+        <v>84</v>
+      </c>
+      <c r="B84" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="C84" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="13">
+        <v>85</v>
+      </c>
+      <c r="B85" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C85" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="13">
+        <v>86</v>
+      </c>
+      <c r="B86" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C86" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="13">
+        <v>87</v>
+      </c>
+      <c r="B87" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="C87" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="13">
+        <v>88</v>
+      </c>
+      <c r="B88" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C88" s="21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="13">
+        <v>89</v>
+      </c>
+      <c r="B89" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="C89" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="13">
+        <v>90</v>
+      </c>
+      <c r="B90" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="C90" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="13">
+        <v>91</v>
+      </c>
+      <c r="B91" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C91" s="21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="13">
+        <v>92</v>
+      </c>
+      <c r="B92" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="C92" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="13">
+        <v>93</v>
+      </c>
+      <c r="B93" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="C93" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="13">
+        <v>94</v>
+      </c>
+      <c r="B94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C94" s="21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="13">
+        <v>95</v>
+      </c>
+      <c r="B95" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C95" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="13">
+        <v>96</v>
+      </c>
+      <c r="B96" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="C96" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="13">
+        <v>97</v>
+      </c>
+      <c r="B97" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="C97" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="13">
+        <v>98</v>
+      </c>
+      <c r="B98" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="C98" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="13">
+        <v>99</v>
+      </c>
+      <c r="B99" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="C99" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="13">
+        <v>100</v>
+      </c>
+      <c r="B100" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="C100" s="21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="13">
+        <v>101</v>
+      </c>
+      <c r="B101" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="C101" s="21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="13">
+        <v>102</v>
+      </c>
+      <c r="B102" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="C102" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="13">
+        <v>103</v>
+      </c>
+      <c r="B103" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="C103" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C1:C103 A1:B60">
+    <cfRule type="expression" dxfId="1" priority="5">
+      <formula>$C1=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61:C103">
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>$C61=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61:C103">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C103">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>